<commit_message>
Version 1.1 add new feature
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\printing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778D372E-C9E9-41D9-8CBD-DB6BF81DD50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A477C6F-D1D5-4F14-A8D3-4843A5ED2616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -1878,7 +1878,7 @@
     <t>ГБУЗ НСО  НКЦРБ</t>
   </si>
   <si>
-    <t>None</t>
+    <t>Номер эталона в госреестре</t>
   </si>
 </sst>
 </file>
@@ -2687,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M211"/>
+  <dimension ref="A1:M210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,6 +2798,9 @@
       <c r="G9" t="s">
         <v>10</v>
       </c>
+      <c r="H9" t="s">
+        <v>614</v>
+      </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
@@ -11053,11 +11056,6 @@
       </c>
       <c r="M210">
         <v>100.3</v>
-      </c>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 1.6 add new row type
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88572C5B-EC64-4056-A653-CA3EE9C40A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0AC2A3-8E79-49B8-BAF6-21782B38647B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="375" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -7290,7 +7290,7 @@
   <dimension ref="A1:P202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15612,7 +15612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FA6792-25B0-4D78-A4D1-DB70E82B7D80}">
   <dimension ref="A1:M449"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17147,7 +17147,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="95">
         <v>45159</v>
       </c>
@@ -17188,7 +17188,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="95">
         <v>45159</v>
       </c>
@@ -17229,7 +17229,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="95">
         <v>45159</v>
       </c>
@@ -17270,7 +17270,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="95">
         <v>45159</v>
       </c>
@@ -20468,7 +20468,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="95">
         <v>45173</v>
       </c>
@@ -20509,7 +20509,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A120" s="95">
         <v>45173</v>
       </c>
@@ -20550,7 +20550,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A121" s="95">
         <v>45173</v>
       </c>
@@ -20591,7 +20591,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A122" s="95">
         <v>45173</v>
       </c>
@@ -20632,7 +20632,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A123" s="95">
         <v>45173</v>
       </c>
@@ -20673,7 +20673,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A124" s="95">
         <v>45173</v>
       </c>
@@ -20714,7 +20714,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A125" s="95">
         <v>45173</v>
       </c>
@@ -20755,7 +20755,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A126" s="95">
         <v>45173</v>
       </c>
@@ -21903,7 +21903,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A154" s="95">
         <v>45195</v>
       </c>
@@ -21944,7 +21944,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="95">
         <v>45195</v>
       </c>
@@ -21985,7 +21985,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="95">
         <v>45195</v>
       </c>
@@ -22026,7 +22026,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A157" s="95">
         <v>45195</v>
       </c>
@@ -22272,7 +22272,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="95">
         <v>45195</v>
       </c>
@@ -22477,7 +22477,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="95">
         <v>45196</v>
       </c>
@@ -22518,7 +22518,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A169" s="95">
         <v>45196</v>
       </c>
@@ -22559,7 +22559,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A170" s="95">
         <v>45196</v>
       </c>
@@ -27725,7 +27725,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="296" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A296" s="95">
         <v>45202</v>
       </c>
@@ -27889,7 +27889,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="300" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A300" s="95">
         <v>45202</v>
       </c>
@@ -27930,7 +27930,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="301" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A301" s="95">
         <v>45202</v>
       </c>
@@ -27971,7 +27971,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="302" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A302" s="95">
         <v>45202</v>
       </c>
@@ -28012,7 +28012,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="303" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A303" s="95">
         <v>45202</v>
       </c>
@@ -28053,7 +28053,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="304" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A304" s="95">
         <v>45202</v>
       </c>
@@ -28094,7 +28094,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="305" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A305" s="95">
         <v>45202</v>
       </c>
@@ -28545,7 +28545,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="316" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A316" s="95">
         <v>45207</v>
       </c>
@@ -28586,7 +28586,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="317" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A317" s="95">
         <v>45207</v>
       </c>
@@ -28627,7 +28627,7 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="318" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A318" s="95">
         <v>45207</v>
       </c>
@@ -28668,7 +28668,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="319" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A319" s="95">
         <v>45207</v>
       </c>
@@ -28709,7 +28709,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="320" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A320" s="95">
         <v>45207</v>
       </c>
@@ -29037,7 +29037,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="328" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A328" s="95">
         <v>45208</v>
       </c>
@@ -29078,7 +29078,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="329" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A329" s="95">
         <v>45208</v>
       </c>
@@ -29201,7 +29201,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="332" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A332" s="95">
         <v>45208</v>
       </c>
@@ -32481,7 +32481,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="412" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A412" s="95">
         <v>45195</v>
       </c>
@@ -32522,7 +32522,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="413" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A413" s="95">
         <v>45195</v>
       </c>
@@ -32563,7 +32563,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="414" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A414" s="95">
         <v>45195</v>
       </c>

</xml_diff>

<commit_message>
Version 2.1.1b minor fix bug
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\printing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB1A92D-E7E3-44BD-AFDF-C340251CAFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E3B9F0-6B58-4E29-B684-2C220C9D2E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7290,7 +7290,7 @@
   <dimension ref="A1:R202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>